<commit_message>
Fix bug generating c# table assertions from excel
This is a missing bit of logic after commit f45ff33. The fact that
both of these have to be in sync is a code smell.

This code compiles, and I think the test generation is ok now as
well. Now need to implement the test.
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
+++ b/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F3893471-4A7E-4473-AB89-20619D3AF3B6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{57D2F6FA-BD0A-4B52-94CC-C2FECA42EEB9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="19035" windowHeight="10635" tabRatio="752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -309,389 +309,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="59">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -1132,14 +750,15 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="13" customWidth="1"/>
     <col min="2" max="2" width="37" style="13" customWidth="1"/>
-    <col min="3" max="4" width="18.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="13" customWidth="1"/>
     <col min="5" max="5" width="22" style="13" customWidth="1"/>
     <col min="6" max="6" width="24.140625" style="13" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" style="13" customWidth="1"/>
@@ -1393,7 +1012,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
         <v>39</v>
       </c>
@@ -1409,7 +1028,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D24" s="13" t="s">
         <v>43</v>
       </c>
@@ -1419,7 +1038,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D26" s="13" t="s">
         <v>42</v>
       </c>
@@ -1461,7 +1080,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D28" s="13">
-        <f t="shared" ref="C28:D34" si="0">O28*N28/M28</f>
+        <f t="shared" ref="D28:D34" si="0">O28*N28/M28</f>
         <v>140.01601451311993</v>
       </c>
       <c r="F28" s="13">
@@ -1469,15 +1088,15 @@
         <v>38</v>
       </c>
       <c r="G28" s="13">
-        <f>F11* (2 * PI() / 60)</f>
+        <f t="shared" ref="G28:G34" si="2">F11* (2 * PI() / 60)</f>
         <v>1.5707963267948966</v>
       </c>
       <c r="H28" s="13">
-        <f>(G28 * F28) /D11</f>
+        <f t="shared" ref="H28:H34" si="3">(G28 * F28) /D11</f>
         <v>5.9690260418206069</v>
       </c>
       <c r="I28" s="13">
-        <f>IF(G11&gt;0.8888,3,1/SQRT(1-G11))</f>
+        <f t="shared" ref="I28:I34" si="4">IF(G11&gt;0.8888,3,1/SQRT(1-G11))</f>
         <v>1.8257418583505536</v>
       </c>
       <c r="J28" s="13">
@@ -1485,11 +1104,11 @@
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K28" s="13">
-        <f>IF(E11&gt;0.02,2.5*E11+0.05,5*E11)</f>
+        <f t="shared" ref="K28:K34" si="5">IF(E11&gt;0.02,2.5*E11+0.05,5*E11)</f>
         <v>0.42499999999999999</v>
       </c>
       <c r="L28" s="13">
-        <f>0.012*H11*H28</f>
+        <f t="shared" ref="L28:L34" si="6">0.012*H11*H28</f>
         <v>0.21488493750554188</v>
       </c>
       <c r="M28" s="13">
@@ -1497,11 +1116,11 @@
         <v>0.47934634550188976</v>
       </c>
       <c r="N28" s="13">
-        <f t="shared" ref="N28:N34" si="2">F28*SQRT((I28+1)/2)</f>
+        <f t="shared" ref="N28:N34" si="7">F28*SQRT((I28+1)/2)</f>
         <v>45.168413982882988</v>
       </c>
       <c r="O28" s="13">
-        <f t="shared" ref="O28:O34" si="3">SQRT(0.214+0.144*I28)* (1-SQRT(0.134+0.124*I28))/((1-SQRT(0.214+0.144*I28))*SQRT(0.134+0.124*I28))</f>
+        <f t="shared" ref="O28:O34" si="8">SQRT(0.214+0.144*I28)* (1-SQRT(0.134+0.124*I28))/((1-SQRT(0.214+0.144*I28))*SQRT(0.134+0.124*I28))</f>
         <v>1.4859092660202307</v>
       </c>
     </row>
@@ -1515,39 +1134,39 @@
         <v>38</v>
       </c>
       <c r="G29" s="13">
-        <f>F12* (2 * PI() / 60)</f>
+        <f t="shared" si="2"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="H29" s="13">
-        <f>(G29 * F29) /D12</f>
+        <f t="shared" si="3"/>
         <v>5.9690260418206069</v>
       </c>
       <c r="I29" s="13">
-        <f>IF(G12&gt;0.8888,3,1/SQRT(1-G12))</f>
+        <f t="shared" si="4"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="J29" s="13">
-        <f t="shared" ref="J29:J34" si="4">(1-I29)*SQRT(1.49+I29)/(9.76*(1+I29))</f>
+        <f t="shared" ref="J29:J34" si="9">(1-I29)*SQRT(1.49+I29)/(9.76*(1+I29))</f>
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K29" s="13">
-        <f>IF(E12&gt;0.02,2.5*E12+0.05,5*E12)</f>
+        <f t="shared" si="5"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="L29" s="13">
-        <f>0.012*H12*H29</f>
+        <f t="shared" si="6"/>
         <v>0.14325662500369457</v>
       </c>
       <c r="M29" s="13">
-        <f t="shared" ref="M29:M34" si="5">SQRT(POWER(J29,2)+POWER(K29,2)+POWER(L29,2))</f>
+        <f t="shared" ref="M29:M34" si="10">SQRT(POWER(J29,2)+POWER(K29,2)+POWER(L29,2))</f>
         <v>0.45179624078416769</v>
       </c>
       <c r="N29" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>45.168413982882988</v>
       </c>
       <c r="O29" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
     </row>
@@ -1561,39 +1180,39 @@
         <v>38</v>
       </c>
       <c r="G30" s="13">
-        <f>F13* (2 * PI() / 60)</f>
+        <f t="shared" si="2"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="H30" s="13">
-        <f>(G30 * F30) /D13</f>
+        <f t="shared" si="3"/>
         <v>9.9483767363676776</v>
       </c>
       <c r="I30" s="13">
-        <f>IF(G13&gt;0.8888,3,1/SQRT(1-G13))</f>
+        <f t="shared" si="4"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="J30" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K30" s="13">
-        <f>IF(E13&gt;0.02,2.5*E13+0.05,5*E13)</f>
+        <f t="shared" si="5"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="L30" s="13">
-        <f>0.012*H13*H30</f>
+        <f t="shared" si="6"/>
         <v>0.35814156250923646</v>
       </c>
       <c r="M30" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.55844673996345773</v>
       </c>
       <c r="N30" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>45.168413982882988</v>
       </c>
       <c r="O30" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
     </row>
@@ -1607,39 +1226,39 @@
         <v>38</v>
       </c>
       <c r="G31" s="13">
-        <f>F14* (2 * PI() / 60)</f>
+        <f t="shared" si="2"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="H31" s="13">
-        <f>(G31 * F31) /D14</f>
+        <f t="shared" si="3"/>
         <v>5.9690260418206069</v>
       </c>
       <c r="I31" s="13">
-        <f>IF(G14&gt;0.8888,3,1/SQRT(1-G14))</f>
+        <f t="shared" si="4"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="J31" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K31" s="13">
-        <f>IF(E14&gt;0.02,2.5*E14+0.05,5*E14)</f>
+        <f t="shared" si="5"/>
         <v>0.3</v>
       </c>
       <c r="L31" s="13">
-        <f>0.012*H14*H31</f>
+        <f t="shared" si="6"/>
         <v>0.21488493750554188</v>
       </c>
       <c r="M31" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.37302535965536859</v>
       </c>
       <c r="N31" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>45.168413982882988</v>
       </c>
       <c r="O31" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
     </row>
@@ -1653,39 +1272,39 @@
         <v>30</v>
       </c>
       <c r="G32" s="13">
-        <f>F15* (2 * PI() / 60)</f>
+        <f t="shared" si="2"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="H32" s="13">
-        <f>(G32 * F32) /D15</f>
+        <f t="shared" si="3"/>
         <v>4.7123889803846897</v>
       </c>
       <c r="I32" s="13">
-        <f>IF(G15&gt;0.8888,3,1/SQRT(1-G15))</f>
+        <f t="shared" si="4"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="J32" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K32" s="13">
-        <f>IF(E15&gt;0.02,2.5*E15+0.05,5*E15)</f>
+        <f t="shared" si="5"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="L32" s="13">
-        <f>0.012*H15*H32</f>
+        <f t="shared" si="6"/>
         <v>0.16964600329384885</v>
       </c>
       <c r="M32" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.46084395299584113</v>
       </c>
       <c r="N32" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>35.659274197012884</v>
       </c>
       <c r="O32" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
     </row>
@@ -1699,39 +1318,39 @@
         <v>38</v>
       </c>
       <c r="G33" s="13">
-        <f>F16* (2 * PI() / 60)</f>
+        <f t="shared" si="2"/>
         <v>2.0943951023931953</v>
       </c>
       <c r="H33" s="13">
-        <f>(G33 * F33) /D16</f>
+        <f t="shared" si="3"/>
         <v>7.9587013890941423</v>
       </c>
       <c r="I33" s="13">
-        <f>IF(G16&gt;0.8888,3,1/SQRT(1-G16))</f>
+        <f t="shared" si="4"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="J33" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K33" s="13">
-        <f>IF(E16&gt;0.02,2.5*E16+0.05,5*E16)</f>
+        <f t="shared" si="5"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="L33" s="13">
-        <f>0.012*H16*H33</f>
+        <f t="shared" si="6"/>
         <v>0.28651325000738914</v>
       </c>
       <c r="M33" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.51544856679309248</v>
       </c>
       <c r="N33" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>45.168413982882988</v>
       </c>
       <c r="O33" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
     </row>
@@ -1745,87 +1364,87 @@
         <v>38</v>
       </c>
       <c r="G34" s="13">
-        <f>F17* (2 * PI() / 60)</f>
+        <f t="shared" si="2"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="H34" s="13">
-        <f>(G34 * F34) /D17</f>
+        <f t="shared" si="3"/>
         <v>5.9690260418206069</v>
       </c>
       <c r="I34" s="13">
-        <f>IF(G17&gt;0.8888,3,1/SQRT(1-G17))</f>
+        <f t="shared" si="4"/>
         <v>1.5811388300841895</v>
       </c>
       <c r="J34" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>-4.0426713559809861E-2</v>
       </c>
       <c r="K34" s="13">
-        <f>IF(E17&gt;0.02,2.5*E17+0.05,5*E17)</f>
+        <f t="shared" si="5"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="L34" s="13">
-        <f>0.012*H17*H34</f>
+        <f t="shared" si="6"/>
         <v>0.21488493750554188</v>
       </c>
       <c r="M34" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.47794859089237574</v>
       </c>
       <c r="N34" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>43.169227874966502</v>
       </c>
       <c r="O34" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>1.4674942789516103</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="58" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="54" priority="8" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="8" priority="8" operator="beginsWith" text="With Properties">
       <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="53" priority="9" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="7" priority="9" operator="endsWith" text=" table of">
       <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="52" priority="10" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="6" priority="10" operator="endsWith" text=" of">
       <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="11">
+    <cfRule type="expression" dxfId="5" priority="11">
       <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="12">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="13">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="46" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implement the vermuelen near wake length caclulation logic
The new test now passes on my computer.
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
+++ b/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{57D2F6FA-BD0A-4B52-94CC-C2FECA42EEB9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EED1B4C5-E48F-4E86-A429-5B4C86DB84D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="19035" windowHeight="10635" tabRatio="752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Diameter</t>
   </si>
@@ -101,9 +101,6 @@
     <t>VermeulenNearWakeLengthInputs table of</t>
   </si>
   <si>
-    <t>VermeulenNearWakeLengthInputs</t>
-  </si>
-  <si>
     <t>TurbineGeometry of</t>
   </si>
   <si>
@@ -159,6 +156,15 @@
   </si>
   <si>
     <t>Spaces in the Excel filename</t>
+  </si>
+  <si>
+    <t>VermeulenNearWakeLengthInput</t>
+  </si>
+  <si>
+    <t>Ambient Turbulence Wake Erosion Rate</t>
+  </si>
+  <si>
+    <t>Helper worksheets that do not get converted in to tests</t>
   </si>
 </sst>
 </file>
@@ -749,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A4AB2E-8077-4D7F-985C-A2ECF36784A5}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +771,7 @@
     <col min="8" max="8" width="20.85546875" style="13" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" style="13" customWidth="1"/>
     <col min="10" max="10" width="34" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="35.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" style="13" customWidth="1"/>
     <col min="12" max="12" width="29.28515625" style="13" customWidth="1"/>
     <col min="13" max="13" width="18.85546875" style="13" customWidth="1"/>
     <col min="14" max="14" width="36" style="13" bestFit="1" customWidth="1"/>
@@ -781,15 +787,15 @@
         <v>20</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="L2" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -800,7 +806,7 @@
         <v>21</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -808,7 +814,7 @@
         <v>19</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -816,7 +822,10 @@
         <v>25</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>26</v>
+        <v>45</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -835,15 +844,15 @@
         <v>24</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H8" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -853,10 +862,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1001,26 +1010,26 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>40</v>
-      </c>
       <c r="D22" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1030,20 +1039,20 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D24" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D25" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D26" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="D27" s="13">
         <v>1E-3</v>
       </c>
@@ -1063,7 +1072,7 @@
         <v>6</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="L27" s="13" t="s">
         <v>4</v>
@@ -1080,23 +1089,23 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D28" s="13">
-        <f t="shared" ref="D28:D34" si="0">O28*N28/M28</f>
+        <f>O28*N28/M28</f>
         <v>140.01601451311993</v>
       </c>
       <c r="F28" s="13">
-        <f t="shared" ref="F28:F34" si="1">I11/2</f>
+        <f t="shared" ref="F28:F34" si="0">I11/2</f>
         <v>38</v>
       </c>
       <c r="G28" s="13">
-        <f t="shared" ref="G28:G34" si="2">F11* (2 * PI() / 60)</f>
+        <f t="shared" ref="G28:G34" si="1">F11* (2 * PI() / 60)</f>
         <v>1.5707963267948966</v>
       </c>
       <c r="H28" s="13">
-        <f t="shared" ref="H28:H34" si="3">(G28 * F28) /D11</f>
+        <f t="shared" ref="H28:H34" si="2">(G28 * F28) /D11</f>
         <v>5.9690260418206069</v>
       </c>
       <c r="I28" s="13">
-        <f t="shared" ref="I28:I34" si="4">IF(G11&gt;0.8888,3,1/SQRT(1-G11))</f>
+        <f t="shared" ref="I28:I34" si="3">IF(G11&gt;0.8888,3,1/SQRT(1-G11))</f>
         <v>1.8257418583505536</v>
       </c>
       <c r="J28" s="13">
@@ -1104,11 +1113,11 @@
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K28" s="13">
-        <f t="shared" ref="K28:K34" si="5">IF(E11&gt;0.02,2.5*E11+0.05,5*E11)</f>
+        <f t="shared" ref="K28:K34" si="4">IF(E11&gt;0.02,2.5*E11+0.05,5*E11)</f>
         <v>0.42499999999999999</v>
       </c>
       <c r="L28" s="13">
-        <f t="shared" ref="L28:L34" si="6">0.012*H11*H28</f>
+        <f t="shared" ref="L28:L34" si="5">0.012*H11*H28</f>
         <v>0.21488493750554188</v>
       </c>
       <c r="M28" s="13">
@@ -1116,33 +1125,33 @@
         <v>0.47934634550188976</v>
       </c>
       <c r="N28" s="13">
-        <f t="shared" ref="N28:N34" si="7">F28*SQRT((I28+1)/2)</f>
+        <f t="shared" ref="N28:N34" si="6">F28*SQRT((I28+1)/2)</f>
         <v>45.168413982882988</v>
       </c>
       <c r="O28" s="13">
-        <f t="shared" ref="O28:O34" si="8">SQRT(0.214+0.144*I28)* (1-SQRT(0.134+0.124*I28))/((1-SQRT(0.214+0.144*I28))*SQRT(0.134+0.124*I28))</f>
+        <f t="shared" ref="O28:O34" si="7">SQRT(0.214+0.144*I28)* (1-SQRT(0.134+0.124*I28))/((1-SQRT(0.214+0.144*I28))*SQRT(0.134+0.124*I28))</f>
         <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D29" s="13">
+        <f t="shared" ref="D28:D34" si="8">O29*N29/M29</f>
+        <v>148.55405780294296</v>
+      </c>
+      <c r="F29" s="13">
         <f t="shared" si="0"/>
-        <v>148.55405780294296</v>
-      </c>
-      <c r="F29" s="13">
+        <v>38</v>
+      </c>
+      <c r="G29" s="13">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="G29" s="13">
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="H29" s="13">
         <f t="shared" si="2"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="H29" s="13">
+        <v>5.9690260418206069</v>
+      </c>
+      <c r="I29" s="13">
         <f t="shared" si="3"/>
-        <v>5.9690260418206069</v>
-      </c>
-      <c r="I29" s="13">
-        <f t="shared" si="4"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="J29" s="13">
@@ -1150,11 +1159,11 @@
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K29" s="13">
+        <f t="shared" si="4"/>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="L29" s="13">
         <f t="shared" si="5"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L29" s="13">
-        <f t="shared" si="6"/>
         <v>0.14325662500369457</v>
       </c>
       <c r="M29" s="13">
@@ -1162,33 +1171,33 @@
         <v>0.45179624078416769</v>
       </c>
       <c r="N29" s="13">
+        <f t="shared" si="6"/>
+        <v>45.168413982882988</v>
+      </c>
+      <c r="O29" s="13">
         <f t="shared" si="7"/>
-        <v>45.168413982882988</v>
-      </c>
-      <c r="O29" s="13">
-        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D30" s="13">
+        <f t="shared" si="8"/>
+        <v>120.18364521743895</v>
+      </c>
+      <c r="F30" s="13">
         <f t="shared" si="0"/>
-        <v>120.18364521743895</v>
-      </c>
-      <c r="F30" s="13">
+        <v>38</v>
+      </c>
+      <c r="G30" s="13">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="G30" s="13">
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="H30" s="13">
         <f t="shared" si="2"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="H30" s="13">
+        <v>9.9483767363676776</v>
+      </c>
+      <c r="I30" s="13">
         <f t="shared" si="3"/>
-        <v>9.9483767363676776</v>
-      </c>
-      <c r="I30" s="13">
-        <f t="shared" si="4"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="J30" s="13">
@@ -1196,11 +1205,11 @@
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K30" s="13">
+        <f t="shared" si="4"/>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="L30" s="13">
         <f t="shared" si="5"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L30" s="13">
-        <f t="shared" si="6"/>
         <v>0.35814156250923646</v>
       </c>
       <c r="M30" s="13">
@@ -1208,33 +1217,33 @@
         <v>0.55844673996345773</v>
       </c>
       <c r="N30" s="13">
+        <f t="shared" si="6"/>
+        <v>45.168413982882988</v>
+      </c>
+      <c r="O30" s="13">
         <f t="shared" si="7"/>
-        <v>45.168413982882988</v>
-      </c>
-      <c r="O30" s="13">
-        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D31" s="13">
+        <f t="shared" si="8"/>
+        <v>179.92386611626353</v>
+      </c>
+      <c r="F31" s="13">
         <f t="shared" si="0"/>
-        <v>179.92386611626353</v>
-      </c>
-      <c r="F31" s="13">
+        <v>38</v>
+      </c>
+      <c r="G31" s="13">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="G31" s="13">
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="H31" s="13">
         <f t="shared" si="2"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="H31" s="13">
+        <v>5.9690260418206069</v>
+      </c>
+      <c r="I31" s="13">
         <f t="shared" si="3"/>
-        <v>5.9690260418206069</v>
-      </c>
-      <c r="I31" s="13">
-        <f t="shared" si="4"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="J31" s="13">
@@ -1242,11 +1251,11 @@
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K31" s="13">
+        <f t="shared" si="4"/>
+        <v>0.3</v>
+      </c>
+      <c r="L31" s="13">
         <f t="shared" si="5"/>
-        <v>0.3</v>
-      </c>
-      <c r="L31" s="13">
-        <f t="shared" si="6"/>
         <v>0.21488493750554188</v>
       </c>
       <c r="M31" s="13">
@@ -1254,33 +1263,33 @@
         <v>0.37302535965536859</v>
       </c>
       <c r="N31" s="13">
+        <f t="shared" si="6"/>
+        <v>45.168413982882988</v>
+      </c>
+      <c r="O31" s="13">
         <f t="shared" si="7"/>
-        <v>45.168413982882988</v>
-      </c>
-      <c r="O31" s="13">
-        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D32" s="13">
+        <f t="shared" si="8"/>
+        <v>114.97697996131835</v>
+      </c>
+      <c r="F32" s="13">
         <f t="shared" si="0"/>
-        <v>114.97697996131835</v>
-      </c>
-      <c r="F32" s="13">
+        <v>30</v>
+      </c>
+      <c r="G32" s="13">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="G32" s="13">
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="H32" s="13">
         <f t="shared" si="2"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="H32" s="13">
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="I32" s="13">
         <f t="shared" si="3"/>
-        <v>4.7123889803846897</v>
-      </c>
-      <c r="I32" s="13">
-        <f t="shared" si="4"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="J32" s="13">
@@ -1288,11 +1297,11 @@
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K32" s="13">
+        <f t="shared" si="4"/>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="L32" s="13">
         <f t="shared" si="5"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L32" s="13">
-        <f t="shared" si="6"/>
         <v>0.16964600329384885</v>
       </c>
       <c r="M32" s="13">
@@ -1300,33 +1309,33 @@
         <v>0.46084395299584113</v>
       </c>
       <c r="N32" s="13">
+        <f t="shared" si="6"/>
+        <v>35.659274197012884</v>
+      </c>
+      <c r="O32" s="13">
         <f t="shared" si="7"/>
-        <v>35.659274197012884</v>
-      </c>
-      <c r="O32" s="13">
-        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="33" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D33" s="13">
+        <f t="shared" si="8"/>
+        <v>130.2092375310549</v>
+      </c>
+      <c r="F33" s="13">
         <f t="shared" si="0"/>
-        <v>130.2092375310549</v>
-      </c>
-      <c r="F33" s="13">
+        <v>38</v>
+      </c>
+      <c r="G33" s="13">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="G33" s="13">
+        <v>2.0943951023931953</v>
+      </c>
+      <c r="H33" s="13">
         <f t="shared" si="2"/>
-        <v>2.0943951023931953</v>
-      </c>
-      <c r="H33" s="13">
+        <v>7.9587013890941423</v>
+      </c>
+      <c r="I33" s="13">
         <f t="shared" si="3"/>
-        <v>7.9587013890941423</v>
-      </c>
-      <c r="I33" s="13">
-        <f t="shared" si="4"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="J33" s="13">
@@ -1334,11 +1343,11 @@
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="K33" s="13">
+        <f t="shared" si="4"/>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="L33" s="13">
         <f t="shared" si="5"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L33" s="13">
-        <f t="shared" si="6"/>
         <v>0.28651325000738914</v>
       </c>
       <c r="M33" s="13">
@@ -1346,33 +1355,33 @@
         <v>0.51544856679309248</v>
       </c>
       <c r="N33" s="13">
+        <f t="shared" si="6"/>
+        <v>45.168413982882988</v>
+      </c>
+      <c r="O33" s="13">
         <f t="shared" si="7"/>
-        <v>45.168413982882988</v>
-      </c>
-      <c r="O33" s="13">
-        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="34" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D34" s="13">
+        <f t="shared" si="8"/>
+        <v>132.54688085802303</v>
+      </c>
+      <c r="F34" s="13">
         <f t="shared" si="0"/>
-        <v>132.54688085802303</v>
-      </c>
-      <c r="F34" s="13">
+        <v>38</v>
+      </c>
+      <c r="G34" s="13">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="G34" s="13">
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="H34" s="13">
         <f t="shared" si="2"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="H34" s="13">
+        <v>5.9690260418206069</v>
+      </c>
+      <c r="I34" s="13">
         <f t="shared" si="3"/>
-        <v>5.9690260418206069</v>
-      </c>
-      <c r="I34" s="13">
-        <f t="shared" si="4"/>
         <v>1.5811388300841895</v>
       </c>
       <c r="J34" s="13">
@@ -1380,11 +1389,11 @@
         <v>-4.0426713559809861E-2</v>
       </c>
       <c r="K34" s="13">
+        <f t="shared" si="4"/>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="L34" s="13">
         <f t="shared" si="5"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L34" s="13">
-        <f t="shared" si="6"/>
         <v>0.21488493750554188</v>
       </c>
       <c r="M34" s="13">
@@ -1392,11 +1401,11 @@
         <v>0.47794859089237574</v>
       </c>
       <c r="N34" s="13">
+        <f t="shared" si="6"/>
+        <v>43.169227874966502</v>
+      </c>
+      <c r="O34" s="13">
         <f t="shared" si="7"/>
-        <v>43.169227874966502</v>
-      </c>
-      <c r="O34" s="13">
-        <f t="shared" si="8"/>
         <v>1.4674942789516103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add more detail to the assertions and use named ranges in excel
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
+++ b/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EED1B4C5-E48F-4E86-A429-5B4C86DB84D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AFC57278-C514-4A7A-B2B5-D5B7791C1679}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="19035" windowHeight="10635" tabRatio="752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,25 @@
     <sheet name="VermeulenNearWakeLength" sheetId="8" r:id="rId1"/>
     <sheet name="Original Calc" sheetId="7" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="AmbientTurbulenceWakeErosionRate">VermeulenNearWakeLength!$I$28:$I$34</definedName>
+    <definedName name="AngularVelocity">VermeulenNearWakeLength!$E$28:$E$34</definedName>
+    <definedName name="FlowFieldRatio">VermeulenNearWakeLength!$G$28:$G$34</definedName>
+    <definedName name="MechanicalWakeErosionRate">VermeulenNearWakeLength!$J$28:$J$34</definedName>
+    <definedName name="N">VermeulenNearWakeLength!$M$28:$M$34</definedName>
+    <definedName name="Radius">VermeulenNearWakeLength!$O$28:$O$34</definedName>
+    <definedName name="RadiusOfInviscidExpandedRotorDisk">VermeulenNearWakeLength!$L$28:$L$34</definedName>
+    <definedName name="ShearTurbulenceWakeErosionRate">VermeulenNearWakeLength!$H$28:$H$34</definedName>
+    <definedName name="ThrustCoefficient">VermeulenNearWakeLength!$G$28:$G$34</definedName>
+    <definedName name="TipSpeedRatio">VermeulenNearWakeLength!$F$28:$F$34</definedName>
+    <definedName name="TotalErosionRate">VermeulenNearWakeLength!$K$28:$K$34</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>Diameter</t>
   </si>
@@ -161,10 +174,34 @@
     <t>VermeulenNearWakeLengthInput</t>
   </si>
   <si>
-    <t>Ambient Turbulence Wake Erosion Rate</t>
-  </si>
-  <si>
     <t>Helper worksheets that do not get converted in to tests</t>
+  </si>
+  <si>
+    <t>Using named ranges in calculations</t>
+  </si>
+  <si>
+    <t>AngularVelocity</t>
+  </si>
+  <si>
+    <t>TipSpeedRatio</t>
+  </si>
+  <si>
+    <t>FlowFieldRatio</t>
+  </si>
+  <si>
+    <t>ShearTurbulenceWakeErosionRate</t>
+  </si>
+  <si>
+    <t>AmbientTurbulenceWakeErosionRate</t>
+  </si>
+  <si>
+    <t>MechanicalWakeErosionRate</t>
+  </si>
+  <si>
+    <t>TotalErosionRate</t>
+  </si>
+  <si>
+    <t>RadiusOfInviscidExpandedRotorDisk</t>
   </si>
 </sst>
 </file>
@@ -315,7 +352,1357 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="175">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -755,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A4AB2E-8077-4D7F-985C-A2ECF36784A5}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,12 +2157,13 @@
     <col min="7" max="7" width="19.85546875" style="13" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" style="13" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" style="13" customWidth="1"/>
-    <col min="10" max="10" width="34" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" style="13" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" style="13" customWidth="1"/>
-    <col min="14" max="14" width="36" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="18.85546875" style="13" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" style="13" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="13" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" style="13" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="13" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" style="13" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" style="13" customWidth="1"/>
+    <col min="16" max="18" width="18.85546875" style="13" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
@@ -825,12 +2213,15 @@
         <v>45</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="D6" s="13" t="s">
         <v>19</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1037,424 +2428,1027 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="D24" s="13" t="s">
         <v>42</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D25" s="13" t="s">
         <v>40</v>
       </c>
+      <c r="E25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="D26" s="13" t="s">
         <v>41</v>
       </c>
+      <c r="E26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="27" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D27" s="13">
         <v>1E-3</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="E27" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="F27" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="G27" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="H27" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="I27" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="J27" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="K27" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="L27" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="M27" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="O27" s="13" t="s">
         <v>10</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K27" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="L27" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="M27" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="N27" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="O27" s="13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D28" s="13">
-        <f>O28*N28/M28</f>
+        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
         <v>140.01601451311993</v>
       </c>
+      <c r="E28" s="13">
+        <f>F11* (2 * PI() / 60)</f>
+        <v>1.5707963267948966</v>
+      </c>
       <c r="F28" s="13">
-        <f t="shared" ref="F28:F34" si="0">I11/2</f>
+        <f>(AngularVelocity * Radius) / D11</f>
+        <v>5.9690260418206069</v>
+      </c>
+      <c r="G28" s="13">
+        <f>IF(G11&gt;0.8888,3,1/SQRT(1-G11))</f>
+        <v>1.8257418583505536</v>
+      </c>
+      <c r="H28" s="13">
+        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <v>-5.4519561436758443E-2</v>
+      </c>
+      <c r="I28" s="13">
+        <f>IF(E11&gt;0.02,2.5*E11+0.05,5*E11)</f>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="J28" s="13">
+        <f>0.012*H11*TipSpeedRatio</f>
+        <v>0.21488493750554188</v>
+      </c>
+      <c r="K28" s="13">
+        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <v>0.47934634550188976</v>
+      </c>
+      <c r="L28" s="13">
+        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <v>45.168413982882988</v>
+      </c>
+      <c r="M28" s="13">
+        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <v>1.4859092660202307</v>
+      </c>
+      <c r="O28" s="13">
+        <f>I11/2</f>
         <v>38</v>
-      </c>
-      <c r="G28" s="13">
-        <f t="shared" ref="G28:G34" si="1">F11* (2 * PI() / 60)</f>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="H28" s="13">
-        <f t="shared" ref="H28:H34" si="2">(G28 * F28) /D11</f>
-        <v>5.9690260418206069</v>
-      </c>
-      <c r="I28" s="13">
-        <f t="shared" ref="I28:I34" si="3">IF(G11&gt;0.8888,3,1/SQRT(1-G11))</f>
-        <v>1.8257418583505536</v>
-      </c>
-      <c r="J28" s="13">
-        <f>(1-I28)*SQRT(1.49+I28)/(9.76*(1+I28))</f>
-        <v>-5.4519561436758443E-2</v>
-      </c>
-      <c r="K28" s="13">
-        <f t="shared" ref="K28:K34" si="4">IF(E11&gt;0.02,2.5*E11+0.05,5*E11)</f>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L28" s="13">
-        <f t="shared" ref="L28:L34" si="5">0.012*H11*H28</f>
-        <v>0.21488493750554188</v>
-      </c>
-      <c r="M28" s="13">
-        <f>SQRT(POWER(J28,2)+POWER(K28,2)+POWER(L28,2))</f>
-        <v>0.47934634550188976</v>
-      </c>
-      <c r="N28" s="13">
-        <f t="shared" ref="N28:N34" si="6">F28*SQRT((I28+1)/2)</f>
-        <v>45.168413982882988</v>
-      </c>
-      <c r="O28" s="13">
-        <f t="shared" ref="O28:O34" si="7">SQRT(0.214+0.144*I28)* (1-SQRT(0.134+0.124*I28))/((1-SQRT(0.214+0.144*I28))*SQRT(0.134+0.124*I28))</f>
-        <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D29" s="13">
-        <f t="shared" ref="D28:D34" si="8">O29*N29/M29</f>
+        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
         <v>148.55405780294296</v>
       </c>
+      <c r="E29" s="13">
+        <f>F12* (2 * PI() / 60)</f>
+        <v>1.5707963267948966</v>
+      </c>
       <c r="F29" s="13">
-        <f t="shared" si="0"/>
+        <f>(AngularVelocity * Radius) /D12</f>
+        <v>5.9690260418206069</v>
+      </c>
+      <c r="G29" s="13">
+        <f>IF(G12&gt;0.8888,3,1/SQRT(1-G12))</f>
+        <v>1.8257418583505536</v>
+      </c>
+      <c r="H29" s="13">
+        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <v>-5.4519561436758443E-2</v>
+      </c>
+      <c r="I29" s="13">
+        <f>IF(E12&gt;0.02,2.5*E12+0.05,5*E12)</f>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="J29" s="13">
+        <f>0.012*H12*TipSpeedRatio</f>
+        <v>0.14325662500369457</v>
+      </c>
+      <c r="K29" s="13">
+        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <v>0.45179624078416769</v>
+      </c>
+      <c r="L29" s="13">
+        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <v>45.168413982882988</v>
+      </c>
+      <c r="M29" s="13">
+        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <v>1.4859092660202307</v>
+      </c>
+      <c r="O29" s="13">
+        <f t="shared" ref="O29:O34" si="0">I12/2</f>
         <v>38</v>
-      </c>
-      <c r="G29" s="13">
-        <f t="shared" si="1"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="H29" s="13">
-        <f t="shared" si="2"/>
-        <v>5.9690260418206069</v>
-      </c>
-      <c r="I29" s="13">
-        <f t="shared" si="3"/>
-        <v>1.8257418583505536</v>
-      </c>
-      <c r="J29" s="13">
-        <f t="shared" ref="J29:J34" si="9">(1-I29)*SQRT(1.49+I29)/(9.76*(1+I29))</f>
-        <v>-5.4519561436758443E-2</v>
-      </c>
-      <c r="K29" s="13">
-        <f t="shared" si="4"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L29" s="13">
-        <f t="shared" si="5"/>
-        <v>0.14325662500369457</v>
-      </c>
-      <c r="M29" s="13">
-        <f t="shared" ref="M29:M34" si="10">SQRT(POWER(J29,2)+POWER(K29,2)+POWER(L29,2))</f>
-        <v>0.45179624078416769</v>
-      </c>
-      <c r="N29" s="13">
-        <f t="shared" si="6"/>
-        <v>45.168413982882988</v>
-      </c>
-      <c r="O29" s="13">
-        <f t="shared" si="7"/>
-        <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D30" s="13">
-        <f t="shared" si="8"/>
+        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
         <v>120.18364521743895</v>
       </c>
+      <c r="E30" s="13">
+        <f>F13* (2 * PI() / 60)</f>
+        <v>1.5707963267948966</v>
+      </c>
       <c r="F30" s="13">
+        <f>(AngularVelocity * Radius) /D13</f>
+        <v>9.9483767363676776</v>
+      </c>
+      <c r="G30" s="13">
+        <f>IF(G13&gt;0.8888,3,1/SQRT(1-G13))</f>
+        <v>1.8257418583505536</v>
+      </c>
+      <c r="H30" s="13">
+        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <v>-5.4519561436758443E-2</v>
+      </c>
+      <c r="I30" s="13">
+        <f>IF(E13&gt;0.02,2.5*E13+0.05,5*E13)</f>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="J30" s="13">
+        <f>0.012*H13*TipSpeedRatio</f>
+        <v>0.35814156250923646</v>
+      </c>
+      <c r="K30" s="13">
+        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <v>0.55844673996345773</v>
+      </c>
+      <c r="L30" s="13">
+        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <v>45.168413982882988</v>
+      </c>
+      <c r="M30" s="13">
+        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <v>1.4859092660202307</v>
+      </c>
+      <c r="O30" s="13">
         <f t="shared" si="0"/>
         <v>38</v>
-      </c>
-      <c r="G30" s="13">
-        <f t="shared" si="1"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="H30" s="13">
-        <f t="shared" si="2"/>
-        <v>9.9483767363676776</v>
-      </c>
-      <c r="I30" s="13">
-        <f t="shared" si="3"/>
-        <v>1.8257418583505536</v>
-      </c>
-      <c r="J30" s="13">
-        <f t="shared" si="9"/>
-        <v>-5.4519561436758443E-2</v>
-      </c>
-      <c r="K30" s="13">
-        <f t="shared" si="4"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L30" s="13">
-        <f t="shared" si="5"/>
-        <v>0.35814156250923646</v>
-      </c>
-      <c r="M30" s="13">
-        <f t="shared" si="10"/>
-        <v>0.55844673996345773</v>
-      </c>
-      <c r="N30" s="13">
-        <f t="shared" si="6"/>
-        <v>45.168413982882988</v>
-      </c>
-      <c r="O30" s="13">
-        <f t="shared" si="7"/>
-        <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D31" s="13">
-        <f t="shared" si="8"/>
+        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
         <v>179.92386611626353</v>
       </c>
+      <c r="E31" s="13">
+        <f>F14* (2 * PI() / 60)</f>
+        <v>1.5707963267948966</v>
+      </c>
       <c r="F31" s="13">
+        <f>(AngularVelocity * Radius) /D14</f>
+        <v>5.9690260418206069</v>
+      </c>
+      <c r="G31" s="13">
+        <f>IF(G14&gt;0.8888,3,1/SQRT(1-G14))</f>
+        <v>1.8257418583505536</v>
+      </c>
+      <c r="H31" s="13">
+        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <v>-5.4519561436758443E-2</v>
+      </c>
+      <c r="I31" s="13">
+        <f>IF(E14&gt;0.02,2.5*E14+0.05,5*E14)</f>
+        <v>0.3</v>
+      </c>
+      <c r="J31" s="13">
+        <f>0.012*H14*TipSpeedRatio</f>
+        <v>0.21488493750554188</v>
+      </c>
+      <c r="K31" s="13">
+        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <v>0.37302535965536859</v>
+      </c>
+      <c r="L31" s="13">
+        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <v>45.168413982882988</v>
+      </c>
+      <c r="M31" s="13">
+        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <v>1.4859092660202307</v>
+      </c>
+      <c r="O31" s="13">
         <f t="shared" si="0"/>
         <v>38</v>
-      </c>
-      <c r="G31" s="13">
-        <f t="shared" si="1"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="H31" s="13">
-        <f t="shared" si="2"/>
-        <v>5.9690260418206069</v>
-      </c>
-      <c r="I31" s="13">
-        <f t="shared" si="3"/>
-        <v>1.8257418583505536</v>
-      </c>
-      <c r="J31" s="13">
-        <f t="shared" si="9"/>
-        <v>-5.4519561436758443E-2</v>
-      </c>
-      <c r="K31" s="13">
-        <f t="shared" si="4"/>
-        <v>0.3</v>
-      </c>
-      <c r="L31" s="13">
-        <f t="shared" si="5"/>
-        <v>0.21488493750554188</v>
-      </c>
-      <c r="M31" s="13">
-        <f t="shared" si="10"/>
-        <v>0.37302535965536859</v>
-      </c>
-      <c r="N31" s="13">
-        <f t="shared" si="6"/>
-        <v>45.168413982882988</v>
-      </c>
-      <c r="O31" s="13">
-        <f t="shared" si="7"/>
-        <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D32" s="13">
-        <f t="shared" si="8"/>
+        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
         <v>114.97697996131835</v>
       </c>
+      <c r="E32" s="13">
+        <f>F15* (2 * PI() / 60)</f>
+        <v>1.5707963267948966</v>
+      </c>
       <c r="F32" s="13">
+        <f>(AngularVelocity * Radius) /D15</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="G32" s="13">
+        <f>IF(G15&gt;0.8888,3,1/SQRT(1-G15))</f>
+        <v>1.8257418583505536</v>
+      </c>
+      <c r="H32" s="13">
+        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <v>-5.4519561436758443E-2</v>
+      </c>
+      <c r="I32" s="13">
+        <f>IF(E15&gt;0.02,2.5*E15+0.05,5*E15)</f>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="J32" s="13">
+        <f>0.012*H15*TipSpeedRatio</f>
+        <v>0.16964600329384885</v>
+      </c>
+      <c r="K32" s="13">
+        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <v>0.46084395299584113</v>
+      </c>
+      <c r="L32" s="13">
+        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <v>35.659274197012884</v>
+      </c>
+      <c r="M32" s="13">
+        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <v>1.4859092660202307</v>
+      </c>
+      <c r="O32" s="13">
         <f t="shared" si="0"/>
         <v>30</v>
-      </c>
-      <c r="G32" s="13">
-        <f t="shared" si="1"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="H32" s="13">
-        <f t="shared" si="2"/>
-        <v>4.7123889803846897</v>
-      </c>
-      <c r="I32" s="13">
-        <f t="shared" si="3"/>
-        <v>1.8257418583505536</v>
-      </c>
-      <c r="J32" s="13">
-        <f t="shared" si="9"/>
-        <v>-5.4519561436758443E-2</v>
-      </c>
-      <c r="K32" s="13">
-        <f t="shared" si="4"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L32" s="13">
-        <f t="shared" si="5"/>
-        <v>0.16964600329384885</v>
-      </c>
-      <c r="M32" s="13">
-        <f t="shared" si="10"/>
-        <v>0.46084395299584113</v>
-      </c>
-      <c r="N32" s="13">
-        <f t="shared" si="6"/>
-        <v>35.659274197012884</v>
-      </c>
-      <c r="O32" s="13">
-        <f t="shared" si="7"/>
-        <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="33" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D33" s="13">
-        <f t="shared" si="8"/>
+        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
         <v>130.2092375310549</v>
       </c>
+      <c r="E33" s="13">
+        <f>F16* (2 * PI() / 60)</f>
+        <v>2.0943951023931953</v>
+      </c>
       <c r="F33" s="13">
+        <f>(AngularVelocity * Radius) /D16</f>
+        <v>7.9587013890941423</v>
+      </c>
+      <c r="G33" s="13">
+        <f>IF(G16&gt;0.8888,3,1/SQRT(1-G16))</f>
+        <v>1.8257418583505536</v>
+      </c>
+      <c r="H33" s="13">
+        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <v>-5.4519561436758443E-2</v>
+      </c>
+      <c r="I33" s="13">
+        <f>IF(E16&gt;0.02,2.5*E16+0.05,5*E16)</f>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="J33" s="13">
+        <f>0.012*H16*TipSpeedRatio</f>
+        <v>0.28651325000738914</v>
+      </c>
+      <c r="K33" s="13">
+        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <v>0.51544856679309248</v>
+      </c>
+      <c r="L33" s="13">
+        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <v>45.168413982882988</v>
+      </c>
+      <c r="M33" s="13">
+        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <v>1.4859092660202307</v>
+      </c>
+      <c r="O33" s="13">
         <f t="shared" si="0"/>
         <v>38</v>
-      </c>
-      <c r="G33" s="13">
-        <f t="shared" si="1"/>
-        <v>2.0943951023931953</v>
-      </c>
-      <c r="H33" s="13">
-        <f t="shared" si="2"/>
-        <v>7.9587013890941423</v>
-      </c>
-      <c r="I33" s="13">
-        <f t="shared" si="3"/>
-        <v>1.8257418583505536</v>
-      </c>
-      <c r="J33" s="13">
-        <f t="shared" si="9"/>
-        <v>-5.4519561436758443E-2</v>
-      </c>
-      <c r="K33" s="13">
-        <f t="shared" si="4"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L33" s="13">
-        <f t="shared" si="5"/>
-        <v>0.28651325000738914</v>
-      </c>
-      <c r="M33" s="13">
-        <f t="shared" si="10"/>
-        <v>0.51544856679309248</v>
-      </c>
-      <c r="N33" s="13">
-        <f t="shared" si="6"/>
-        <v>45.168413982882988</v>
-      </c>
-      <c r="O33" s="13">
-        <f t="shared" si="7"/>
-        <v>1.4859092660202307</v>
       </c>
     </row>
     <row r="34" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D34" s="13">
-        <f t="shared" si="8"/>
+        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
         <v>132.54688085802303</v>
       </c>
+      <c r="E34" s="13">
+        <f>F17* (2 * PI() / 60)</f>
+        <v>1.5707963267948966</v>
+      </c>
       <c r="F34" s="13">
+        <f>(AngularVelocity * Radius) /D17</f>
+        <v>5.9690260418206069</v>
+      </c>
+      <c r="G34" s="13">
+        <f>IF(G17&gt;0.8888,3,1/SQRT(1-G17))</f>
+        <v>1.5811388300841895</v>
+      </c>
+      <c r="H34" s="13">
+        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <v>-4.0426713559809861E-2</v>
+      </c>
+      <c r="I34" s="13">
+        <f>IF(E17&gt;0.02,2.5*E17+0.05,5*E17)</f>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="J34" s="13">
+        <f>0.012*H17*TipSpeedRatio</f>
+        <v>0.21488493750554188</v>
+      </c>
+      <c r="K34" s="13">
+        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <v>0.47794859089237574</v>
+      </c>
+      <c r="L34" s="13">
+        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <v>43.169227874966502</v>
+      </c>
+      <c r="M34" s="13">
+        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <v>1.4674942789516103</v>
+      </c>
+      <c r="O34" s="13">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="G34" s="13">
-        <f t="shared" si="1"/>
-        <v>1.5707963267948966</v>
-      </c>
-      <c r="H34" s="13">
-        <f t="shared" si="2"/>
-        <v>5.9690260418206069</v>
-      </c>
-      <c r="I34" s="13">
-        <f t="shared" si="3"/>
-        <v>1.5811388300841895</v>
-      </c>
-      <c r="J34" s="13">
-        <f t="shared" si="9"/>
-        <v>-4.0426713559809861E-2</v>
-      </c>
-      <c r="K34" s="13">
-        <f t="shared" si="4"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="L34" s="13">
-        <f t="shared" si="5"/>
-        <v>0.21488493750554188</v>
-      </c>
-      <c r="M34" s="13">
-        <f t="shared" si="10"/>
-        <v>0.47794859089237574</v>
-      </c>
-      <c r="N34" s="13">
-        <f t="shared" si="6"/>
-        <v>43.169227874966502</v>
-      </c>
-      <c r="O34" s="13">
-        <f t="shared" si="7"/>
-        <v>1.4674942789516103</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+  <conditionalFormatting sqref="A1:D26 E25:M27 K19:K22 E1:J22 K1:K8 A35:D1048576 E36:XFD1048576 N1:XFD25 L1:M22 P28:XFD33 B27:D34">
+    <cfRule type="cellIs" dxfId="174" priority="4" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="5" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="6" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="7" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="8" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="170" priority="8" operator="beginsWith" text="With Properties">
       <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="7" priority="9" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="169" priority="9" operator="endsWith" text=" table of">
       <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="6" priority="10" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="168" priority="10" operator="endsWith" text=" of">
       <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="11">
+    <cfRule type="expression" dxfId="167" priority="11">
       <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="12">
+    <cfRule type="expression" dxfId="166" priority="12">
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="13">
+  <conditionalFormatting sqref="A1:XFD9 A10:J17 L10:XFD17 A18:XFD1048576">
+    <cfRule type="notContainsBlanks" dxfId="165" priority="13">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="A1:XFD9 A10:J17 L10:XFD17 A18:XFD1048576">
+    <cfRule type="cellIs" dxfId="164" priority="2" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="3" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:XFD9 A10:J17 L10:XFD17 A18:XFD1048576">
+    <cfRule type="cellIs" dxfId="162" priority="1" operator="equal">
       <formula>"StringFormat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q35 E35 K18">
+    <cfRule type="cellIs" dxfId="161" priority="41" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="42" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="159" priority="43" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="44" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="157" priority="45" operator="beginsWith" text="With Properties">
+      <formula>LEFT(E18,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="156" priority="46" operator="endsWith" text=" table of">
+      <formula>RIGHT(E18,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="155" priority="47" operator="endsWith" text=" of">
+      <formula>RIGHT(E18,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="154" priority="48">
+      <formula>AND((RIGHT(#REF!, 3) = " of"), E19 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="153" priority="49">
+      <formula>AND(RIGHT(D18, 3) = " of", E19 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q26 E23:M23 K9">
+    <cfRule type="cellIs" dxfId="152" priority="59" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="60" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="61" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="62" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="148" priority="63" operator="beginsWith" text="With Properties">
+      <formula>LEFT(E9,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="147" priority="64" operator="endsWith" text=" table of">
+      <formula>RIGHT(E9,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="146" priority="65" operator="endsWith" text=" of">
+      <formula>RIGHT(E9,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="145" priority="66">
+      <formula>AND((RIGHT(E8, 3) = " of"), #REF! = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="144" priority="67">
+      <formula>AND(RIGHT(D9, 3) = " of", #REF! = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:A34">
+    <cfRule type="cellIs" dxfId="143" priority="113" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="114" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="115" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="116" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="139" priority="117" operator="beginsWith" text="With Properties">
+      <formula>LEFT(A27,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="138" priority="118" operator="endsWith" text=" table of">
+      <formula>RIGHT(A27,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="137" priority="119" operator="endsWith" text=" of">
+      <formula>RIGHT(A27,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="120">
+      <formula>AND((RIGHT(A26, 3) = " of"), A28 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="135" priority="121">
+      <formula>AND(RIGHT(XFB27, 3) = " of", A28 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N27">
+    <cfRule type="cellIs" dxfId="134" priority="131" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="132" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="133" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="134" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="130" priority="135" operator="beginsWith" text="With Properties">
+      <formula>LEFT(N27,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="129" priority="136" operator="endsWith" text=" table of">
+      <formula>RIGHT(N27,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="128" priority="137" operator="endsWith" text=" of">
+      <formula>RIGHT(N27,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="127" priority="138">
+      <formula>AND((RIGHT(P26, 3) = " of"), N28 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="139">
+      <formula>AND(RIGHT(#REF!, 3) = " of", N28 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G35:P35 R35:XFD35">
+    <cfRule type="cellIs" dxfId="125" priority="140" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="141" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="142" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="143" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="121" priority="144" operator="beginsWith" text="With Properties">
+      <formula>LEFT(G35,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="120" priority="145" operator="endsWith" text=" table of">
+      <formula>RIGHT(G35,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="119" priority="146" operator="endsWith" text=" of">
+      <formula>RIGHT(G35,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="147">
+      <formula>AND((RIGHT(E34, 3) = " of"), G36 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="148">
+      <formula>AND(RIGHT(F35, 3) = " of", G36 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R26:XFD26">
+    <cfRule type="cellIs" dxfId="116" priority="149" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="115" priority="150" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="151" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="152" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="112" priority="153" operator="beginsWith" text="With Properties">
+      <formula>LEFT(R26,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="111" priority="154" operator="endsWith" text=" table of">
+      <formula>RIGHT(R26,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="110" priority="155" operator="endsWith" text=" of">
+      <formula>RIGHT(R26,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="109" priority="156">
+      <formula>AND((RIGHT(R25, 3) = " of"), P27 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="157">
+      <formula>AND(RIGHT(Q26, 3) = " of", P27 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34:N34">
+    <cfRule type="cellIs" dxfId="107" priority="158" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="159" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="160" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="161" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="103" priority="162" operator="beginsWith" text="With Properties">
+      <formula>LEFT(E34,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="102" priority="163" operator="endsWith" text=" table of">
+      <formula>RIGHT(E34,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="101" priority="164" operator="endsWith" text=" of">
+      <formula>RIGHT(E34,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="165">
+      <formula>AND((RIGHT(E33, 3) = " of"), G35 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="99" priority="166">
+      <formula>AND(RIGHT(#REF!, 3) = " of", G35 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N28:N33 E29:M33">
+    <cfRule type="cellIs" dxfId="98" priority="167" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="168" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="169" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="170" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="94" priority="171" operator="beginsWith" text="With Properties">
+      <formula>LEFT(E28,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="93" priority="172" operator="endsWith" text=" table of">
+      <formula>RIGHT(E28,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="92" priority="173" operator="endsWith" text=" of">
+      <formula>RIGHT(E28,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="174">
+      <formula>AND((RIGHT(E27, 3) = " of"), E29 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="90" priority="175">
+      <formula>AND(RIGHT(#REF!, 3) = " of", E29 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O28:O34">
+    <cfRule type="cellIs" dxfId="89" priority="293" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="294" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="295" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="296" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="85" priority="297" operator="beginsWith" text="With Properties">
+      <formula>LEFT(O28,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="84" priority="298" operator="endsWith" text=" table of">
+      <formula>RIGHT(O28,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="83" priority="299" operator="endsWith" text=" of">
+      <formula>RIGHT(O28,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="82" priority="300">
+      <formula>AND((RIGHT(O27, 3) = " of"), O29 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="301">
+      <formula>AND(RIGHT(#REF!, 3) = " of", O29 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24:M24">
+    <cfRule type="cellIs" dxfId="80" priority="373" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="374" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="375" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="376" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="76" priority="377" operator="beginsWith" text="With Properties">
+      <formula>LEFT(E24,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="75" priority="378" operator="endsWith" text=" table of">
+      <formula>RIGHT(E24,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="74" priority="379" operator="endsWith" text=" of">
+      <formula>RIGHT(E24,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="73" priority="380">
+      <formula>AND((RIGHT(G26, 3) = " of"), E28 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="381">
+      <formula>AND(RIGHT(#REF!, 3) = " of", E28 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N26:P26">
+    <cfRule type="cellIs" dxfId="71" priority="382" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="383" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="384" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="385" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="67" priority="386" operator="beginsWith" text="With Properties">
+      <formula>LEFT(N26,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="66" priority="387" operator="endsWith" text=" table of">
+      <formula>RIGHT(N26,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="65" priority="388" operator="endsWith" text=" of">
+      <formula>RIGHT(N26,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="389">
+      <formula>AND((RIGHT(N25, 3) = " of"), L24 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="390">
+      <formula>AND(RIGHT(M26, 3) = " of", L24 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28:M28 F29:F34 H29:H34 J29:M34">
+    <cfRule type="cellIs" dxfId="62" priority="400" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="401" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="402" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="403" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="58" priority="404" operator="beginsWith" text="With Properties">
+      <formula>LEFT(E28,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="57" priority="405" operator="endsWith" text=" table of">
+      <formula>RIGHT(E28,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="56" priority="406" operator="endsWith" text=" of">
+      <formula>RIGHT(E28,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="407">
+      <formula>AND((RIGHT(E24, 3) = " of"), E29 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="54" priority="408">
+      <formula>AND(RIGHT(#REF!, 3) = " of", E29 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O34">
+    <cfRule type="cellIs" dxfId="53" priority="677" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="678" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="679" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="680" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="49" priority="681" operator="beginsWith" text="With Properties">
+      <formula>LEFT(O34,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="48" priority="682" operator="endsWith" text=" table of">
+      <formula>RIGHT(O34,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="47" priority="683" operator="endsWith" text=" of">
+      <formula>RIGHT(O34,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="684">
+      <formula>AND((RIGHT(O33, 3) = " of"), K18 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="685">
+      <formula>AND(RIGHT(#REF!, 3) = " of", K18 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P27:XFD27">
+    <cfRule type="cellIs" dxfId="44" priority="713" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="714" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="715" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="716" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="40" priority="717" operator="beginsWith" text="With Properties">
+      <formula>LEFT(P27,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="39" priority="718" operator="endsWith" text=" table of">
+      <formula>RIGHT(P27,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="38" priority="719" operator="endsWith" text=" of">
+      <formula>RIGHT(P27,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="720">
+      <formula>AND((RIGHT(R26, 3) = " of"), P28 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="721">
+      <formula>AND(RIGHT(O27, 3) = " of", P28 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P34:XFD34">
+    <cfRule type="cellIs" dxfId="35" priority="722" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="723" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="724" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="725" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="31" priority="726" operator="beginsWith" text="With Properties">
+      <formula>LEFT(P34,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="30" priority="727" operator="endsWith" text=" table of">
+      <formula>RIGHT(P34,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="29" priority="728" operator="endsWith" text=" of">
+      <formula>RIGHT(P34,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="729">
+      <formula>AND((RIGHT(P33, 3) = " of"), R35 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="730">
+      <formula>AND(RIGHT(O34, 3) = " of", R35 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O27">
+    <cfRule type="cellIs" dxfId="26" priority="731" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="732" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="733" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="734" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="22" priority="735" operator="beginsWith" text="With Properties">
+      <formula>LEFT(O27,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="21" priority="736" operator="endsWith" text=" table of">
+      <formula>RIGHT(O27,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="20" priority="737" operator="endsWith" text=" of">
+      <formula>RIGHT(O27,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="738">
+      <formula>AND((RIGHT(F26, 3) = " of"), O28 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="739">
+      <formula>AND(RIGHT(#REF!, 3) = " of", O28 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35">
+    <cfRule type="cellIs" dxfId="17" priority="740" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="741" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="742" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="743" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="13" priority="744" operator="beginsWith" text="With Properties">
+      <formula>LEFT(F35,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="12" priority="745" operator="endsWith" text=" table of">
+      <formula>RIGHT(F35,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="11" priority="746" operator="endsWith" text=" of">
+      <formula>RIGHT(F35,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="747">
+      <formula>AND((RIGHT(O34, 3) = " of"), F36 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="748">
+      <formula>AND(RIGHT(E35, 3) = " of", F36 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O34">
+    <cfRule type="cellIs" dxfId="8" priority="749" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="750" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="751" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="752" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="753" operator="beginsWith" text="With Properties">
+      <formula>LEFT(O34,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="3" priority="754" operator="endsWith" text=" table of">
+      <formula>RIGHT(O34,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="2" priority="755" operator="endsWith" text=" of">
+      <formula>RIGHT(O34,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="756">
+      <formula>AND((RIGHT(O33, 3) = " of"), F35 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="757">
+      <formula>AND(RIGHT(#REF!, 3) = " of", F35 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add units to vermuelen near wake length test
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
+++ b/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AFC57278-C514-4A7A-B2B5-D5B7791C1679}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4DAA6570-7298-4613-8229-5DF0D5DDCE04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="19035" windowHeight="10635" tabRatio="752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Diameter</t>
   </si>
@@ -180,9 +180,6 @@
     <t>Using named ranges in calculations</t>
   </si>
   <si>
-    <t>AngularVelocity</t>
-  </si>
-  <si>
     <t>TipSpeedRatio</t>
   </si>
   <si>
@@ -201,7 +198,13 @@
     <t>TotalErosionRate</t>
   </si>
   <si>
-    <t>RadiusOfInviscidExpandedRotorDisk</t>
+    <t>AngularVelocity_rps</t>
+  </si>
+  <si>
+    <t>RadiusOfInviscidExpandedRotorDisk_m</t>
+  </si>
+  <si>
+    <t>Radius_m</t>
   </si>
 </sst>
 </file>
@@ -2142,8 +2145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A4AB2E-8077-4D7F-985C-A2ECF36784A5}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2157,12 +2160,12 @@
     <col min="7" max="7" width="19.85546875" style="13" customWidth="1"/>
     <col min="8" max="8" width="20.85546875" style="13" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" style="13" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="20" style="13" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="13" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" style="13" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" style="13" customWidth="1"/>
     <col min="14" max="14" width="9.7109375" style="13" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="13" customWidth="1"/>
     <col min="16" max="18" width="18.85546875" style="13" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="13"/>
   </cols>
@@ -2433,25 +2436,25 @@
         <v>42</v>
       </c>
       <c r="E24" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="G24" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="H24" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="I24" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="I24" s="13" t="s">
+      <c r="J24" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="K24" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>54</v>
       </c>
       <c r="L24" s="13" t="s">
         <v>55</v>
@@ -2492,7 +2495,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="13" t="s">
         <v>41</v>
       </c>
@@ -2524,7 +2527,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D27" s="13">
         <v>1E-3</v>
       </c>
@@ -2556,16 +2559,16 @@
         <v>1E-3</v>
       </c>
       <c r="O27" s="13" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D28" s="13">
-        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
+        <f t="shared" ref="D28:D34" si="0">N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
         <v>140.01601451311993</v>
       </c>
       <c r="E28" s="13">
-        <f>F11* (2 * PI() / 60)</f>
+        <f t="shared" ref="E28:E34" si="1">F11* (2 * PI() / 60)</f>
         <v>1.5707963267948966</v>
       </c>
       <c r="F28" s="13">
@@ -2573,31 +2576,31 @@
         <v>5.9690260418206069</v>
       </c>
       <c r="G28" s="13">
-        <f>IF(G11&gt;0.8888,3,1/SQRT(1-G11))</f>
+        <f t="shared" ref="G28:G34" si="2">IF(G11&gt;0.8888,3,1/SQRT(1-G11))</f>
         <v>1.8257418583505536</v>
       </c>
       <c r="H28" s="13">
-        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <f t="shared" ref="H28:H34" si="3">(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="I28" s="13">
-        <f>IF(E11&gt;0.02,2.5*E11+0.05,5*E11)</f>
+        <f t="shared" ref="I28:I34" si="4">IF(E11&gt;0.02,2.5*E11+0.05,5*E11)</f>
         <v>0.42499999999999999</v>
       </c>
       <c r="J28" s="13">
-        <f>0.012*H11*TipSpeedRatio</f>
+        <f t="shared" ref="J28:J34" si="5">0.012*H11*TipSpeedRatio</f>
         <v>0.21488493750554188</v>
       </c>
       <c r="K28" s="13">
-        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <f t="shared" ref="K28:K34" si="6">SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
         <v>0.47934634550188976</v>
       </c>
       <c r="L28" s="13">
-        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <f t="shared" ref="L28:L34" si="7">Radius*SQRT((FlowFieldRatio+1)/2)</f>
         <v>45.168413982882988</v>
       </c>
       <c r="M28" s="13">
-        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <f t="shared" ref="M28:M34" si="8">SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
         <v>1.4859092660202307</v>
       </c>
       <c r="O28" s="13">
@@ -2607,277 +2610,277 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D29" s="13">
-        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
+        <f t="shared" si="0"/>
         <v>148.55405780294296</v>
       </c>
       <c r="E29" s="13">
-        <f>F12* (2 * PI() / 60)</f>
+        <f t="shared" si="1"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="F29" s="13">
-        <f>(AngularVelocity * Radius) /D12</f>
+        <f t="shared" ref="F29:F34" si="9">(AngularVelocity * Radius) /D12</f>
         <v>5.9690260418206069</v>
       </c>
       <c r="G29" s="13">
-        <f>IF(G12&gt;0.8888,3,1/SQRT(1-G12))</f>
+        <f t="shared" si="2"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="H29" s="13">
-        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <f t="shared" si="3"/>
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="I29" s="13">
-        <f>IF(E12&gt;0.02,2.5*E12+0.05,5*E12)</f>
+        <f t="shared" si="4"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="J29" s="13">
-        <f>0.012*H12*TipSpeedRatio</f>
+        <f t="shared" si="5"/>
         <v>0.14325662500369457</v>
       </c>
       <c r="K29" s="13">
-        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <f t="shared" si="6"/>
         <v>0.45179624078416769</v>
       </c>
       <c r="L29" s="13">
-        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <f t="shared" si="7"/>
         <v>45.168413982882988</v>
       </c>
       <c r="M29" s="13">
-        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
       <c r="O29" s="13">
-        <f t="shared" ref="O29:O34" si="0">I12/2</f>
+        <f t="shared" ref="O29:O34" si="10">I12/2</f>
         <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D30" s="13">
-        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
+        <f t="shared" si="0"/>
         <v>120.18364521743895</v>
       </c>
       <c r="E30" s="13">
-        <f>F13* (2 * PI() / 60)</f>
+        <f t="shared" si="1"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="F30" s="13">
-        <f>(AngularVelocity * Radius) /D13</f>
+        <f t="shared" si="9"/>
         <v>9.9483767363676776</v>
       </c>
       <c r="G30" s="13">
-        <f>IF(G13&gt;0.8888,3,1/SQRT(1-G13))</f>
+        <f t="shared" si="2"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="H30" s="13">
-        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <f t="shared" si="3"/>
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="I30" s="13">
-        <f>IF(E13&gt;0.02,2.5*E13+0.05,5*E13)</f>
+        <f t="shared" si="4"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="J30" s="13">
-        <f>0.012*H13*TipSpeedRatio</f>
+        <f t="shared" si="5"/>
         <v>0.35814156250923646</v>
       </c>
       <c r="K30" s="13">
-        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <f t="shared" si="6"/>
         <v>0.55844673996345773</v>
       </c>
       <c r="L30" s="13">
-        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <f t="shared" si="7"/>
         <v>45.168413982882988</v>
       </c>
       <c r="M30" s="13">
-        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
       <c r="O30" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D31" s="13">
-        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
+        <f t="shared" si="0"/>
         <v>179.92386611626353</v>
       </c>
       <c r="E31" s="13">
-        <f>F14* (2 * PI() / 60)</f>
+        <f t="shared" si="1"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="F31" s="13">
-        <f>(AngularVelocity * Radius) /D14</f>
+        <f t="shared" si="9"/>
         <v>5.9690260418206069</v>
       </c>
       <c r="G31" s="13">
-        <f>IF(G14&gt;0.8888,3,1/SQRT(1-G14))</f>
+        <f t="shared" si="2"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="H31" s="13">
-        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <f t="shared" si="3"/>
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="I31" s="13">
-        <f>IF(E14&gt;0.02,2.5*E14+0.05,5*E14)</f>
+        <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
       <c r="J31" s="13">
-        <f>0.012*H14*TipSpeedRatio</f>
+        <f t="shared" si="5"/>
         <v>0.21488493750554188</v>
       </c>
       <c r="K31" s="13">
-        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <f t="shared" si="6"/>
         <v>0.37302535965536859</v>
       </c>
       <c r="L31" s="13">
-        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <f t="shared" si="7"/>
         <v>45.168413982882988</v>
       </c>
       <c r="M31" s="13">
-        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
       <c r="O31" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D32" s="13">
-        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
+        <f t="shared" si="0"/>
         <v>114.97697996131835</v>
       </c>
       <c r="E32" s="13">
-        <f>F15* (2 * PI() / 60)</f>
+        <f t="shared" si="1"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="F32" s="13">
-        <f>(AngularVelocity * Radius) /D15</f>
+        <f t="shared" si="9"/>
         <v>4.7123889803846897</v>
       </c>
       <c r="G32" s="13">
-        <f>IF(G15&gt;0.8888,3,1/SQRT(1-G15))</f>
+        <f t="shared" si="2"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="H32" s="13">
-        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <f t="shared" si="3"/>
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="I32" s="13">
-        <f>IF(E15&gt;0.02,2.5*E15+0.05,5*E15)</f>
+        <f t="shared" si="4"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="J32" s="13">
-        <f>0.012*H15*TipSpeedRatio</f>
+        <f t="shared" si="5"/>
         <v>0.16964600329384885</v>
       </c>
       <c r="K32" s="13">
-        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <f t="shared" si="6"/>
         <v>0.46084395299584113</v>
       </c>
       <c r="L32" s="13">
-        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <f t="shared" si="7"/>
         <v>35.659274197012884</v>
       </c>
       <c r="M32" s="13">
-        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
       <c r="O32" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D33" s="13">
-        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
+        <f t="shared" si="0"/>
         <v>130.2092375310549</v>
       </c>
       <c r="E33" s="13">
-        <f>F16* (2 * PI() / 60)</f>
+        <f t="shared" si="1"/>
         <v>2.0943951023931953</v>
       </c>
       <c r="F33" s="13">
-        <f>(AngularVelocity * Radius) /D16</f>
+        <f t="shared" si="9"/>
         <v>7.9587013890941423</v>
       </c>
       <c r="G33" s="13">
-        <f>IF(G16&gt;0.8888,3,1/SQRT(1-G16))</f>
+        <f t="shared" si="2"/>
         <v>1.8257418583505536</v>
       </c>
       <c r="H33" s="13">
-        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <f t="shared" si="3"/>
         <v>-5.4519561436758443E-2</v>
       </c>
       <c r="I33" s="13">
-        <f>IF(E16&gt;0.02,2.5*E16+0.05,5*E16)</f>
+        <f t="shared" si="4"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="J33" s="13">
-        <f>0.012*H16*TipSpeedRatio</f>
+        <f t="shared" si="5"/>
         <v>0.28651325000738914</v>
       </c>
       <c r="K33" s="13">
-        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <f t="shared" si="6"/>
         <v>0.51544856679309248</v>
       </c>
       <c r="L33" s="13">
-        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <f t="shared" si="7"/>
         <v>45.168413982882988</v>
       </c>
       <c r="M33" s="13">
-        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <f t="shared" si="8"/>
         <v>1.4859092660202307</v>
       </c>
       <c r="O33" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>38</v>
       </c>
     </row>
     <row r="34" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D34" s="13">
-        <f>N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
+        <f t="shared" si="0"/>
         <v>132.54688085802303</v>
       </c>
       <c r="E34" s="13">
-        <f>F17* (2 * PI() / 60)</f>
+        <f t="shared" si="1"/>
         <v>1.5707963267948966</v>
       </c>
       <c r="F34" s="13">
-        <f>(AngularVelocity * Radius) /D17</f>
+        <f t="shared" si="9"/>
         <v>5.9690260418206069</v>
       </c>
       <c r="G34" s="13">
-        <f>IF(G17&gt;0.8888,3,1/SQRT(1-G17))</f>
+        <f t="shared" si="2"/>
         <v>1.5811388300841895</v>
       </c>
       <c r="H34" s="13">
-        <f>(1-FlowFieldRatio)*SQRT(1.49+FlowFieldRatio)/(9.76*(1+FlowFieldRatio))</f>
+        <f t="shared" si="3"/>
         <v>-4.0426713559809861E-2</v>
       </c>
       <c r="I34" s="13">
-        <f>IF(E17&gt;0.02,2.5*E17+0.05,5*E17)</f>
+        <f t="shared" si="4"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="J34" s="13">
-        <f>0.012*H17*TipSpeedRatio</f>
+        <f t="shared" si="5"/>
         <v>0.21488493750554188</v>
       </c>
       <c r="K34" s="13">
-        <f>SQRT(POWER(ShearTurbulenceWakeErosionRate,2)+POWER(AmbientTurbulenceWakeErosionRate,2)+POWER(MechanicalWakeErosionRate,2))</f>
+        <f t="shared" si="6"/>
         <v>0.47794859089237574</v>
       </c>
       <c r="L34" s="13">
-        <f>Radius*SQRT((FlowFieldRatio+1)/2)</f>
+        <f t="shared" si="7"/>
         <v>43.169227874966502</v>
       </c>
       <c r="M34" s="13">
-        <f>SQRT(0.214+0.144*FlowFieldRatio)* (1-SQRT(0.134+0.124*FlowFieldRatio))/((1-SQRT(0.214+0.144*FlowFieldRatio))*SQRT(0.134+0.124*FlowFieldRatio))</f>
+        <f t="shared" si="8"/>
         <v>1.4674942789516103</v>
       </c>
       <c r="O34" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="10"/>
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Use Then instead of Assert to match bdd syntax
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
+++ b/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4DAA6570-7298-4613-8229-5DF0D5DDCE04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6F00F9-4530-4EA2-9C30-CE12B91A8D78}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="19035" windowHeight="10635" tabRatio="752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VermeulenNearWakeLength" sheetId="8" r:id="rId1"/>
@@ -29,7 +29,15 @@
     <definedName name="TipSpeedRatio">VermeulenNearWakeLength!$F$28:$F$34</definedName>
     <definedName name="TotalErosionRate">VermeulenNearWakeLength!$K$28:$K$34</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -144,9 +152,6 @@
     <t>Calculate</t>
   </si>
   <si>
-    <t>Assert</t>
-  </si>
-  <si>
     <t>VermeulenNearWakeLength</t>
   </si>
   <si>
@@ -205,6 +210,9 @@
   </si>
   <si>
     <t>Radius_m</t>
+  </si>
+  <si>
+    <t>Then</t>
   </si>
 </sst>
 </file>
@@ -355,7 +363,110 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="175">
+  <dxfs count="188">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2145,8 +2256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A4AB2E-8077-4D7F-985C-A2ECF36784A5}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,7 +2281,7 @@
     <col min="19" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
@@ -2184,7 +2295,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="L2" s="13" t="s">
         <v>32</v>
       </c>
@@ -2197,15 +2308,15 @@
         <v>21</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>19</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2213,10 +2324,10 @@
         <v>25</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2224,7 +2335,7 @@
         <v>19</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2412,18 +2523,18 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>39</v>
-      </c>
       <c r="D22" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2433,31 +2544,31 @@
     </row>
     <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="D24" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="L24" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>55</v>
       </c>
       <c r="M24" s="13" t="s">
         <v>14</v>
@@ -2465,66 +2576,66 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M25" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M26" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2559,7 +2670,7 @@
         <v>1E-3</v>
       </c>
       <c r="O27" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2885,573 +2996,51 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:D26 E25:M27 K19:K22 E1:J22 K1:K8 A35:D1048576 E36:XFD1048576 N1:XFD25 L1:M22 P28:XFD33 B27:D34">
-    <cfRule type="cellIs" dxfId="174" priority="4" operator="equal">
-      <formula>"Assert"</formula>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+      <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="171" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="170" priority="8" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="8" priority="8" operator="beginsWith" text="With Properties">
       <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="169" priority="9" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="7" priority="9" operator="endsWith" text=" table of">
       <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="168" priority="10" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="6" priority="10" operator="endsWith" text=" of">
       <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="11">
+    <cfRule type="expression" dxfId="5" priority="11">
       <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="12">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD9 A10:J17 L10:XFD17 A18:XFD1048576">
-    <cfRule type="notContainsBlanks" dxfId="165" priority="13">
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="13">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD9 A10:J17 L10:XFD17 A18:XFD1048576">
-    <cfRule type="cellIs" dxfId="164" priority="2" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD9 A10:J17 L10:XFD17 A18:XFD1048576">
-    <cfRule type="cellIs" dxfId="162" priority="1" operator="equal">
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"StringFormat"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q35 E35 K18">
-    <cfRule type="cellIs" dxfId="161" priority="41" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="42" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="43" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="44" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="157" priority="45" operator="beginsWith" text="With Properties">
-      <formula>LEFT(E18,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="156" priority="46" operator="endsWith" text=" table of">
-      <formula>RIGHT(E18,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="155" priority="47" operator="endsWith" text=" of">
-      <formula>RIGHT(E18,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="154" priority="48">
-      <formula>AND((RIGHT(#REF!, 3) = " of"), E19 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="153" priority="49">
-      <formula>AND(RIGHT(D18, 3) = " of", E19 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q26 E23:M23 K9">
-    <cfRule type="cellIs" dxfId="152" priority="59" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="60" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="61" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="62" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="148" priority="63" operator="beginsWith" text="With Properties">
-      <formula>LEFT(E9,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="147" priority="64" operator="endsWith" text=" table of">
-      <formula>RIGHT(E9,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="146" priority="65" operator="endsWith" text=" of">
-      <formula>RIGHT(E9,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="145" priority="66">
-      <formula>AND((RIGHT(E8, 3) = " of"), #REF! = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="144" priority="67">
-      <formula>AND(RIGHT(D9, 3) = " of", #REF! = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:A34">
-    <cfRule type="cellIs" dxfId="143" priority="113" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="114" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="115" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="116" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="139" priority="117" operator="beginsWith" text="With Properties">
-      <formula>LEFT(A27,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="138" priority="118" operator="endsWith" text=" table of">
-      <formula>RIGHT(A27,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="137" priority="119" operator="endsWith" text=" of">
-      <formula>RIGHT(A27,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="120">
-      <formula>AND((RIGHT(A26, 3) = " of"), A28 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="135" priority="121">
-      <formula>AND(RIGHT(XFB27, 3) = " of", A28 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N27">
-    <cfRule type="cellIs" dxfId="134" priority="131" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="132" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="133" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="134" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="130" priority="135" operator="beginsWith" text="With Properties">
-      <formula>LEFT(N27,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="129" priority="136" operator="endsWith" text=" table of">
-      <formula>RIGHT(N27,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="128" priority="137" operator="endsWith" text=" of">
-      <formula>RIGHT(N27,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="127" priority="138">
-      <formula>AND((RIGHT(P26, 3) = " of"), N28 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="126" priority="139">
-      <formula>AND(RIGHT(#REF!, 3) = " of", N28 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35:P35 R35:XFD35">
-    <cfRule type="cellIs" dxfId="125" priority="140" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="141" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="142" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="143" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="121" priority="144" operator="beginsWith" text="With Properties">
-      <formula>LEFT(G35,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="120" priority="145" operator="endsWith" text=" table of">
-      <formula>RIGHT(G35,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="119" priority="146" operator="endsWith" text=" of">
-      <formula>RIGHT(G35,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="147">
-      <formula>AND((RIGHT(E34, 3) = " of"), G36 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="117" priority="148">
-      <formula>AND(RIGHT(F35, 3) = " of", G36 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R26:XFD26">
-    <cfRule type="cellIs" dxfId="116" priority="149" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="150" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="151" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="152" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="112" priority="153" operator="beginsWith" text="With Properties">
-      <formula>LEFT(R26,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="111" priority="154" operator="endsWith" text=" table of">
-      <formula>RIGHT(R26,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="110" priority="155" operator="endsWith" text=" of">
-      <formula>RIGHT(R26,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="156">
-      <formula>AND((RIGHT(R25, 3) = " of"), P27 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="108" priority="157">
-      <formula>AND(RIGHT(Q26, 3) = " of", P27 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34:N34">
-    <cfRule type="cellIs" dxfId="107" priority="158" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="159" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="160" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="161" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="103" priority="162" operator="beginsWith" text="With Properties">
-      <formula>LEFT(E34,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="102" priority="163" operator="endsWith" text=" table of">
-      <formula>RIGHT(E34,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="101" priority="164" operator="endsWith" text=" of">
-      <formula>RIGHT(E34,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="165">
-      <formula>AND((RIGHT(E33, 3) = " of"), G35 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="99" priority="166">
-      <formula>AND(RIGHT(#REF!, 3) = " of", G35 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N28:N33 E29:M33">
-    <cfRule type="cellIs" dxfId="98" priority="167" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="168" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="169" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="170" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="94" priority="171" operator="beginsWith" text="With Properties">
-      <formula>LEFT(E28,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="93" priority="172" operator="endsWith" text=" table of">
-      <formula>RIGHT(E28,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="92" priority="173" operator="endsWith" text=" of">
-      <formula>RIGHT(E28,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="174">
-      <formula>AND((RIGHT(E27, 3) = " of"), E29 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="90" priority="175">
-      <formula>AND(RIGHT(#REF!, 3) = " of", E29 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O28:O34">
-    <cfRule type="cellIs" dxfId="89" priority="293" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="294" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="295" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="296" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="85" priority="297" operator="beginsWith" text="With Properties">
-      <formula>LEFT(O28,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="84" priority="298" operator="endsWith" text=" table of">
-      <formula>RIGHT(O28,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="83" priority="299" operator="endsWith" text=" of">
-      <formula>RIGHT(O28,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="300">
-      <formula>AND((RIGHT(O27, 3) = " of"), O29 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="301">
-      <formula>AND(RIGHT(#REF!, 3) = " of", O29 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24:M24">
-    <cfRule type="cellIs" dxfId="80" priority="373" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="374" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="375" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="376" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="76" priority="377" operator="beginsWith" text="With Properties">
-      <formula>LEFT(E24,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="75" priority="378" operator="endsWith" text=" table of">
-      <formula>RIGHT(E24,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="74" priority="379" operator="endsWith" text=" of">
-      <formula>RIGHT(E24,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="380">
-      <formula>AND((RIGHT(G26, 3) = " of"), E28 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="381">
-      <formula>AND(RIGHT(#REF!, 3) = " of", E28 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N26:P26">
-    <cfRule type="cellIs" dxfId="71" priority="382" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="383" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="384" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="385" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="67" priority="386" operator="beginsWith" text="With Properties">
-      <formula>LEFT(N26,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="66" priority="387" operator="endsWith" text=" table of">
-      <formula>RIGHT(N26,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="65" priority="388" operator="endsWith" text=" of">
-      <formula>RIGHT(N26,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="389">
-      <formula>AND((RIGHT(N25, 3) = " of"), L24 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="63" priority="390">
-      <formula>AND(RIGHT(M26, 3) = " of", L24 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28:M28 F29:F34 H29:H34 J29:M34">
-    <cfRule type="cellIs" dxfId="62" priority="400" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="401" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="402" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="403" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="58" priority="404" operator="beginsWith" text="With Properties">
-      <formula>LEFT(E28,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="57" priority="405" operator="endsWith" text=" table of">
-      <formula>RIGHT(E28,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="56" priority="406" operator="endsWith" text=" of">
-      <formula>RIGHT(E28,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="407">
-      <formula>AND((RIGHT(E24, 3) = " of"), E29 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="408">
-      <formula>AND(RIGHT(#REF!, 3) = " of", E29 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O34">
-    <cfRule type="cellIs" dxfId="53" priority="677" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="678" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="679" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="680" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="49" priority="681" operator="beginsWith" text="With Properties">
-      <formula>LEFT(O34,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="48" priority="682" operator="endsWith" text=" table of">
-      <formula>RIGHT(O34,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="47" priority="683" operator="endsWith" text=" of">
-      <formula>RIGHT(O34,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="684">
-      <formula>AND((RIGHT(O33, 3) = " of"), K18 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="685">
-      <formula>AND(RIGHT(#REF!, 3) = " of", K18 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P27:XFD27">
-    <cfRule type="cellIs" dxfId="44" priority="713" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="714" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="715" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="716" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="40" priority="717" operator="beginsWith" text="With Properties">
-      <formula>LEFT(P27,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="39" priority="718" operator="endsWith" text=" table of">
-      <formula>RIGHT(P27,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="38" priority="719" operator="endsWith" text=" of">
-      <formula>RIGHT(P27,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="720">
-      <formula>AND((RIGHT(R26, 3) = " of"), P28 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="721">
-      <formula>AND(RIGHT(O27, 3) = " of", P28 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P34:XFD34">
-    <cfRule type="cellIs" dxfId="35" priority="722" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="723" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="724" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="725" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="31" priority="726" operator="beginsWith" text="With Properties">
-      <formula>LEFT(P34,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="30" priority="727" operator="endsWith" text=" table of">
-      <formula>RIGHT(P34,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="29" priority="728" operator="endsWith" text=" of">
-      <formula>RIGHT(P34,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="729">
-      <formula>AND((RIGHT(P33, 3) = " of"), R35 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="730">
-      <formula>AND(RIGHT(O34, 3) = " of", R35 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O27">
-    <cfRule type="cellIs" dxfId="26" priority="731" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="732" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="733" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="734" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="735" operator="beginsWith" text="With Properties">
-      <formula>LEFT(O27,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="21" priority="736" operator="endsWith" text=" table of">
-      <formula>RIGHT(O27,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="20" priority="737" operator="endsWith" text=" of">
-      <formula>RIGHT(O27,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="738">
-      <formula>AND((RIGHT(F26, 3) = " of"), O28 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="739">
-      <formula>AND(RIGHT(#REF!, 3) = " of", O28 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
-    <cfRule type="cellIs" dxfId="17" priority="740" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="741" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="742" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="743" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="744" operator="beginsWith" text="With Properties">
-      <formula>LEFT(F35,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="12" priority="745" operator="endsWith" text=" table of">
-      <formula>RIGHT(F35,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="11" priority="746" operator="endsWith" text=" of">
-      <formula>RIGHT(F35,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="747">
-      <formula>AND((RIGHT(O34, 3) = " of"), F36 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="748">
-      <formula>AND(RIGHT(E35, 3) = " of", F36 = "With Properties")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O34">
-    <cfRule type="cellIs" dxfId="8" priority="749" operator="equal">
-      <formula>"Assert"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="750" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="751" operator="equal">
-      <formula>"Given a"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="752" operator="equal">
-      <formula>"Specification"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="753" operator="beginsWith" text="With Properties">
-      <formula>LEFT(O34,LEN("With Properties"))="With Properties"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="3" priority="754" operator="endsWith" text=" table of">
-      <formula>RIGHT(O34,LEN(" table of"))=" table of"</formula>
-    </cfRule>
-    <cfRule type="endsWith" dxfId="2" priority="755" operator="endsWith" text=" of">
-      <formula>RIGHT(O34,LEN(" of"))=" of"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="756">
-      <formula>AND((RIGHT(O33, 3) = " of"), F35 = "With Properties")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="757">
-      <formula>AND(RIGHT(#REF!, 3) = " of", F35 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add end to end test for generating setup classes for partial matches
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
+++ b/SampleTests/ExcelTests/Vermeulen Near Wake Length.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6F00F9-4530-4EA2-9C30-CE12B91A8D78}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B18AD8-9872-44BF-935D-2EE1A1337464}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,1460 +363,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="188">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -2260,28 +807,28 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" style="13" customWidth="1"/>
     <col min="2" max="2" width="37" style="13" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="31.54296875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" style="13" customWidth="1"/>
     <col min="5" max="5" width="22" style="13" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="13" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="24.1796875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="20.81640625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" style="13" customWidth="1"/>
     <col min="10" max="10" width="20" style="13" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" style="13" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" style="13" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" style="13" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="13" customWidth="1"/>
-    <col min="16" max="18" width="18.85546875" style="13" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="13"/>
+    <col min="11" max="11" width="19.26953125" style="13" customWidth="1"/>
+    <col min="12" max="12" width="21.7265625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="19.26953125" style="13" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" style="13" customWidth="1"/>
+    <col min="16" max="18" width="18.81640625" style="13" customWidth="1"/>
+    <col min="19" max="16384" width="9.1796875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
@@ -2295,12 +842,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="L2" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>18</v>
       </c>
@@ -2311,7 +858,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>19</v>
       </c>
@@ -2319,7 +866,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C5" s="13" t="s">
         <v>25</v>
       </c>
@@ -2330,7 +877,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D6" s="13" t="s">
         <v>19</v>
       </c>
@@ -2338,7 +885,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="13" t="s">
         <v>22</v>
       </c>
@@ -2355,17 +902,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H8" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H9" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H10" s="13" t="s">
         <v>28</v>
       </c>
@@ -2373,7 +920,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D11" s="13">
         <v>10</v>
       </c>
@@ -2393,7 +940,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D12" s="13">
         <v>10</v>
       </c>
@@ -2413,7 +960,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D13" s="13">
         <v>6</v>
       </c>
@@ -2433,7 +980,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D14" s="13">
         <v>10</v>
       </c>
@@ -2453,7 +1000,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D15" s="13">
         <v>10</v>
       </c>
@@ -2473,7 +1020,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D16" s="13">
         <v>10</v>
       </c>
@@ -2493,7 +1040,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D17" s="13">
         <v>10</v>
       </c>
@@ -2513,7 +1060,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>34</v>
       </c>
@@ -2521,12 +1068,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B22" s="13" t="s">
         <v>37</v>
       </c>
@@ -2537,12 +1084,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D23" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="D24" s="13" t="s">
         <v>41</v>
       </c>
@@ -2574,7 +1121,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D25" s="13" t="s">
         <v>39</v>
       </c>
@@ -2606,7 +1153,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D26" s="13" t="s">
         <v>40</v>
       </c>
@@ -2638,7 +1185,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D27" s="13">
         <v>1E-3</v>
       </c>
@@ -2673,7 +1220,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D28" s="13">
         <f t="shared" ref="D28:D34" si="0">N*RadiusOfInviscidExpandedRotorDisk/TotalErosionRate</f>
         <v>140.01601451311993</v>
@@ -2719,7 +1266,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D29" s="13">
         <f t="shared" si="0"/>
         <v>148.55405780294296</v>
@@ -2765,7 +1312,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D30" s="13">
         <f t="shared" si="0"/>
         <v>120.18364521743895</v>
@@ -2811,7 +1358,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D31" s="13">
         <f t="shared" si="0"/>
         <v>179.92386611626353</v>
@@ -2857,7 +1404,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D32" s="13">
         <f t="shared" si="0"/>
         <v>114.97697996131835</v>
@@ -2903,7 +1450,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D33" s="13">
         <f t="shared" si="0"/>
         <v>130.2092375310549</v>
@@ -2949,7 +1496,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D34" s="13">
         <f t="shared" si="0"/>
         <v>132.54688085802303</v>
@@ -3055,26 +1602,26 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4" customWidth="1"/>
-    <col min="10" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.7265625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="36" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
@@ -3127,7 +1674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B3" s="7">
         <v>3</v>
       </c>
@@ -3191,7 +1738,7 @@
         <v>1.4859092660202307</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -3255,7 +1802,7 @@
         <v>1.4859092660202307</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -3319,7 +1866,7 @@
         <v>1.4859092660202307</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="7">
         <v>3</v>
       </c>
@@ -3383,7 +1930,7 @@
         <v>1.4859092660202307</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" s="7">
         <v>3</v>
       </c>
@@ -3447,7 +1994,7 @@
         <v>1.4859092660202307</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>3</v>
       </c>
@@ -3511,7 +2058,7 @@
         <v>1.4859092660202307</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B9" s="7">
         <v>3</v>
       </c>

</xml_diff>